<commit_message>
Adds support for custom publish key on arrays
</commit_message>
<xml_diff>
--- a/scripts/spreadsheet/Redes e Beaglebones.xlsx
+++ b/scripts/spreadsheet/Redes e Beaglebones.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Archive MKS" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'PVs Redis'!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'PVs Redis'!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
   <si>
     <t xml:space="preserve">ENABLE</t>
   </si>
@@ -57,6 +57,9 @@
     <t xml:space="preserve">Scanrate</t>
   </si>
   <si>
+    <t xml:space="preserve">Pub</t>
+  </si>
+  <si>
     <t xml:space="preserve">Location</t>
   </si>
   <si>
@@ -78,13 +81,10 @@
     <t xml:space="preserve">10.128.0.1</t>
   </si>
   <si>
-    <t xml:space="preserve">EPP rack 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnalogVoltage:AN0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB-04:PU-InjSept:VoltageReference-Mon</t>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float:Test-Mon</t>
   </si>
   <si>
     <t xml:space="preserve">V</t>
@@ -96,16 +96,28 @@
     <t xml:space="preserve">BOO-INJ-SEP</t>
   </si>
   <si>
-    <t xml:space="preserve">SetPointVoltage:AN0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB-04:PU-InjSept:VoltageSetPoint-Mon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BO-01D:PU-InjKckr:VoltageReference-Mon</t>
+    <t xml:space="preserve">Hash:Test-Mon|HashName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hash:Test-Mon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array:Test-Mon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array</t>
   </si>
   <si>
     <t xml:space="preserve">BOO-INJ-KICKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array_put</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArraySubscription</t>
   </si>
   <si>
     <t xml:space="preserve">Agilent 4UHV - Reading</t>
@@ -489,7 +501,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,18 +542,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,7 +580,36 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Hyperlink 1" xfId="20"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006100"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFDFDFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -588,6 +617,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C6E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE4D6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -663,9 +713,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:O28" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:O28"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:P28" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:P28"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="ENABLE"/>
     <tableColumn id="2" name="IP"/>
     <tableColumn id="3" name="Rack"/>
@@ -676,11 +726,12 @@
     <tableColumn id="8" name="Unit"/>
     <tableColumn id="9" name="Type"/>
     <tableColumn id="10" name="Scanrate"/>
-    <tableColumn id="11" name="Location"/>
-    <tableColumn id="12" name="LOLO"/>
-    <tableColumn id="13" name="LOW"/>
-    <tableColumn id="14" name="HIGH"/>
-    <tableColumn id="15" name="HIHI"/>
+    <tableColumn id="11" name="Pub"/>
+    <tableColumn id="12" name="Location"/>
+    <tableColumn id="13" name="LOLO"/>
+    <tableColumn id="14" name="LOW"/>
+    <tableColumn id="15" name="HIGH"/>
+    <tableColumn id="16" name="HIHI"/>
   </tableColumns>
 </table>
 </file>
@@ -690,27 +741,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="G2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,22 +808,25 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>19</v>
@@ -788,22 +843,22 @@
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="20.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>23</v>
@@ -818,33 +873,33 @@
         <v>20</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="20.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
         <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>5</v>
@@ -853,84 +908,115 @@
         <v>20</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="K5" s="7"/>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
-      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
-      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
-      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
-      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
-      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="E15" s="8"/>
-      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
@@ -941,7 +1027,7 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
@@ -953,464 +1039,338 @@
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="E21" s="8"/>
-      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="10"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="10"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="10"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="10"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="10"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="10"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="10"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="10"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="10"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="10"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="10"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="10"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="10"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="10"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="10"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="10"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="10"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="10"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="10"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="10"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="10"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="10"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="C47" s="8"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="10"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="C48" s="8"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="10"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="C49" s="8"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="10"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="C50" s="8"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="10"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="C51" s="8"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="10"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="C52" s="8"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="10"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="C53" s="8"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="10"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="C54" s="8"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="10"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="C55" s="8"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="10"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="C56" s="8"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="10"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="C57" s="8"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="10"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="C58" s="8"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="10"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
       <c r="C59" s="8"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="10"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="C60" s="8"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="10"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="C61" s="8"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="10"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="C62" s="8"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="10"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="C63" s="8"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="10"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="C64" s="8"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="10"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
       <c r="C65" s="8"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="10"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="C66" s="8"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="10"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="10"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="10"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="10"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="10"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="10"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="10"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="10"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="10"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="10"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="10"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="10"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="8"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A77">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1433,7 +1393,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.72"/>
@@ -1446,515 +1406,515 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>34</v>
+      <c r="A2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="16" t="str">
+        <v>43</v>
+      </c>
+      <c r="H2" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A2)</f>
         <v>BO-RA20:VA-SIPC-01:Model-Cte</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>41</v>
+      <c r="A3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="16" t="str">
+        <v>49</v>
+      </c>
+      <c r="G3" s="13" t="str">
         <f aca="false">_xlfn.CONCAT($E3,":",G$1)</f>
         <v>TB-03:VA-SIP20-ED:C4</v>
       </c>
-      <c r="H3" s="16" t="str">
+      <c r="H3" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A3)</f>
         <v>BO-RA20:VA-SIPC-01:SerialNumber-Cte</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>47</v>
+      <c r="A4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="16" t="str">
+        <v>56</v>
+      </c>
+      <c r="H4" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A4)</f>
         <v>BO-RA20:VA-SIPC-01:FanTemperature-Mon</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>54</v>
+      <c r="A5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="16" t="str">
+        <v>63</v>
+      </c>
+      <c r="H5" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A5)</f>
         <v>BO-RA20:VA-SIPC-01:Protect-Mon</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>61</v>
+      <c r="A6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="16" t="e">
+        <v>66</v>
+      </c>
+      <c r="D6" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E6,":",D$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E6" s="16" t="e">
+      <c r="E6" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E6,":",E$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F6" s="16" t="e">
+      <c r="F6" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E6,":",F$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G6" s="16" t="e">
+      <c r="G6" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E6,":",G$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H6" s="16" t="str">
+      <c r="H6" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A6)</f>
         <v>BO-RA20:VA-SIPC-01:Step-Mon</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>64</v>
+      <c r="A7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="16" t="e">
+        <v>69</v>
+      </c>
+      <c r="D7" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E7,":",D$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E7" s="16" t="e">
+      <c r="E7" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E7,":",E$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F7" s="16" t="e">
+      <c r="F7" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E7,":",F$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G7" s="16" t="e">
+      <c r="G7" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E7,":",G$1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H7" s="16" t="str">
+      <c r="H7" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A7)</f>
         <v>BO-RA20:VA-SIPC-01:Unit-RB</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="16" t="str">
+      <c r="A8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A8)</f>
         <v>BO-RA20:VA-SIPC-01:Unit-SP</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="H9" s="16" t="str">
+      <c r="A9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="H9" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A9)</f>
         <v>BO-RA20:VA-SIPC-01:Mode-RB</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="H10" s="16" t="str">
+      <c r="A10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="H10" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(C$2,$A10)</f>
         <v>BO-RA20:VA-SIPC-01:Mode-SP</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17"/>
-      <c r="H11" s="16" t="str">
+      <c r="A11" s="14"/>
+      <c r="H11" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B2)</f>
         <v>TB-01:VA-SIP20-BG:Current-Mon</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17"/>
-      <c r="H12" s="16" t="str">
+      <c r="A12" s="14"/>
+      <c r="H12" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B3)</f>
         <v>TB-01:VA-SIP20-BG:Pressure-Mon</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17"/>
-      <c r="H13" s="16" t="str">
+      <c r="A13" s="14"/>
+      <c r="H13" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B4)</f>
         <v>TB-01:VA-SIP20-BG:Voltage-Mon</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17"/>
-      <c r="F14" s="16"/>
-      <c r="H14" s="16" t="str">
+      <c r="A14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="H14" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B5)</f>
         <v>TB-01:VA-SIP20-BG:HVTemperature-Mon</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="16" t="str">
+      <c r="H15" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B6)</f>
         <v>TB-01:VA-SIP20-BG:ErrorCode-Mon</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="16" t="str">
+      <c r="H16" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B7)</f>
         <v>TB-01:VA-SIP20-BG:SetErrorCode-Mon</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="16" t="str">
+      <c r="H17" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(D$2, $B8)</f>
         <v>TB-01:VA-SIP20-BG:DeviceNumber-RB</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="16" t="str">
+      <c r="H18" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B2)</f>
         <v>TB-01:VA-SIP20-ED:Current-Mon</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="16" t="str">
+      <c r="H19" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B3)</f>
         <v>TB-01:VA-SIP20-ED:Pressure-Mon</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="16" t="str">
+      <c r="H20" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B4)</f>
         <v>TB-01:VA-SIP20-ED:Voltage-Mon</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="16" t="str">
+      <c r="H21" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B5)</f>
         <v>TB-01:VA-SIP20-ED:HVTemperature-Mon</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="16" t="str">
+      <c r="H22" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B6)</f>
         <v>TB-01:VA-SIP20-ED:ErrorCode-Mon</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="16" t="str">
+      <c r="H23" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B7)</f>
         <v>TB-01:VA-SIP20-ED:SetErrorCode-Mon</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="16" t="str">
+      <c r="H24" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(E$2, $B8)</f>
         <v>TB-01:VA-SIP20-ED:DeviceNumber-RB</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="16" t="str">
+      <c r="H25" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B2)</f>
         <v>TB-02:VA-SIP20-BG:Current-Mon</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="16" t="str">
+      <c r="H26" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B3)</f>
         <v>TB-02:VA-SIP20-BG:Pressure-Mon</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="16" t="str">
+      <c r="H27" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B4)</f>
         <v>TB-02:VA-SIP20-BG:Voltage-Mon</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="16" t="str">
+      <c r="H28" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B5)</f>
         <v>TB-02:VA-SIP20-BG:HVTemperature-Mon</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="16" t="str">
+      <c r="H29" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B6)</f>
         <v>TB-02:VA-SIP20-BG:ErrorCode-Mon</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="16" t="str">
+      <c r="H30" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B7)</f>
         <v>TB-02:VA-SIP20-BG:SetErrorCode-Mon</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="16" t="str">
+      <c r="H31" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(F$2, $B8)</f>
         <v>TB-02:VA-SIP20-BG:DeviceNumber-RB</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="16" t="str">
+      <c r="H32" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B2)</f>
         <v>TB-02:VA-SIP20-MD:Current-Mon</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="16" t="str">
+      <c r="H33" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B3)</f>
         <v>TB-02:VA-SIP20-MD:Pressure-Mon</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="16" t="str">
+      <c r="H34" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B4)</f>
         <v>TB-02:VA-SIP20-MD:Voltage-Mon</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="16" t="str">
+      <c r="H35" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B5)</f>
         <v>TB-02:VA-SIP20-MD:HVTemperature-Mon</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="16" t="str">
+      <c r="H36" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B6)</f>
         <v>TB-02:VA-SIP20-MD:ErrorCode-Mon</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="16" t="str">
+      <c r="H37" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B7)</f>
         <v>TB-02:VA-SIP20-MD:SetErrorCode-Mon</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="16" t="str">
+      <c r="H38" s="13" t="str">
         <f aca="false">_xlfn.CONCAT(G$2, $B8)</f>
         <v>TB-02:VA-SIP20-MD:DeviceNumber-RB</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1962,7 +1922,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1982,7 +1942,7 @@
       <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -1996,30 +1956,30 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>30</v>
+      <c r="D1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>5</v>
@@ -2027,32 +1987,32 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="16" t="e">
+        <v>82</v>
+      </c>
+      <c r="E2" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E2,":",E$1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="16" t="e">
+        <v>83</v>
+      </c>
+      <c r="G2" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E2,":",G$1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="16" t="e">
+        <v>84</v>
+      </c>
+      <c r="I2" s="13" t="e">
         <f aca="false">_xlfn.CONCAT($E2,":",I$1)</f>
         <v>#VALUE!</v>
       </c>
@@ -2063,10 +2023,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A3)</f>
@@ -2075,10 +2035,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A4)</f>
@@ -2087,10 +2047,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A5)</f>
@@ -2099,7 +2059,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A6)</f>
@@ -2108,7 +2068,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A7)</f>
@@ -2117,7 +2077,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A8)</f>
@@ -2126,7 +2086,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="K9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A9)</f>
@@ -2135,7 +2095,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A10)</f>
@@ -2144,7 +2104,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A11)</f>
@@ -2153,7 +2113,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="K12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A12)</f>
@@ -2162,7 +2122,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A13)</f>
@@ -2171,7 +2131,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="K14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A14)</f>
@@ -2180,7 +2140,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A15)</f>
@@ -2189,7 +2149,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A16)</f>
@@ -2198,7 +2158,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A17)</f>
@@ -2207,7 +2167,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A18)</f>
@@ -2216,7 +2176,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="K19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A19)</f>
@@ -2225,7 +2185,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="K20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A20)</f>
@@ -2234,7 +2194,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A21)</f>
@@ -2243,7 +2203,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="K22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A22)</f>
@@ -2252,7 +2212,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT($C$2,A23)</f>
@@ -2408,12 +2368,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:I2">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>" "</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>